<commit_message>
Model results matrix-Decision Tree model
</commit_message>
<xml_diff>
--- a/ModelResults.xlsx
+++ b/ModelResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lindgp1\Desktop\UM Bootcamp\Module 20 - Final project\Final-Project-Team-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90550E1-9BD9-4091-BA9D-2AAF9461F33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D2BA06-F880-4F22-933F-D721A3E29B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39255" yWindow="2565" windowWidth="25485" windowHeight="11385" xr2:uid="{061E510B-05AA-44E1-B87A-B493465EE388}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Model</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>SVM</t>
+  </si>
+  <si>
+    <t>Decision Tree</t>
   </si>
 </sst>
 </file>
@@ -409,13 +412,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE94B248-0D51-45CC-A7FD-647A713645B2}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -475,6 +481,26 @@
       </c>
       <c r="F3">
         <v>0.42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.83</v>
+      </c>
+      <c r="D4">
+        <v>0.38</v>
+      </c>
+      <c r="E4">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F4">
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All models, plus correlation
</commit_message>
<xml_diff>
--- a/ModelResults.xlsx
+++ b/ModelResults.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lindgp1\Desktop\UM Bootcamp\Module 20 - Final project\Final-Project-Team-7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21556711-574D-42F1-9E2C-039731A0786F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597FBB8C-9E55-4F1A-A300-3716568B6ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39255" yWindow="2565" windowWidth="25485" windowHeight="11385" activeTab="1" xr2:uid="{061E510B-05AA-44E1-B87A-B493465EE388}"/>
   </bookViews>
   <sheets>
-    <sheet name="Results" sheetId="1" r:id="rId1"/>
-    <sheet name="Importance" sheetId="2" r:id="rId2"/>
+    <sheet name="Red Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Red Importance" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -113,6 +113,27 @@
   </si>
   <si>
     <t>Model 5</t>
+  </si>
+  <si>
+    <t>Gradient Boosted Tree</t>
+  </si>
+  <si>
+    <t>Logisitic-ROS</t>
+  </si>
+  <si>
+    <t>Logistic-SMOTE</t>
+  </si>
+  <si>
+    <t>Logistic-Cluster centroid US</t>
+  </si>
+  <si>
+    <t>Model 9</t>
+  </si>
+  <si>
+    <t>Balanced Random Forest Classifier</t>
+  </si>
+  <si>
+    <t>Easy Ensemble AdaBoos Classifier</t>
   </si>
 </sst>
 </file>
@@ -464,15 +485,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE94B248-0D51-45CC-A7FD-647A713645B2}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -573,6 +594,126 @@
       </c>
       <c r="F5">
         <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>0.89</v>
+      </c>
+      <c r="D6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E6">
+        <v>0.43</v>
+      </c>
+      <c r="F6">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>0.83</v>
+      </c>
+      <c r="D7">
+        <v>0.35</v>
+      </c>
+      <c r="E7">
+        <v>0.9</v>
+      </c>
+      <c r="F7">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8">
+        <v>0.84</v>
+      </c>
+      <c r="D8">
+        <v>0.37</v>
+      </c>
+      <c r="E8">
+        <v>0.92</v>
+      </c>
+      <c r="F8">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9">
+        <v>0.82</v>
+      </c>
+      <c r="D9">
+        <v>0.34</v>
+      </c>
+      <c r="E9">
+        <v>0.88</v>
+      </c>
+      <c r="F9">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>0.84</v>
+      </c>
+      <c r="D10">
+        <v>0.36</v>
+      </c>
+      <c r="E10">
+        <v>0.92</v>
+      </c>
+      <c r="F10">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>0.82</v>
+      </c>
+      <c r="D11">
+        <v>0.33</v>
+      </c>
+      <c r="E11">
+        <v>0.9</v>
+      </c>
+      <c r="F11">
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>
@@ -582,7 +723,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3496ED4D-A2DB-4AD0-8403-2BDE515D8280}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
@@ -595,9 +736,11 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -607,8 +750,11 @@
       <c r="G1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -627,8 +773,14 @@
       <c r="H2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -647,8 +799,14 @@
       <c r="H3">
         <v>0.30651499999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>0.23349900000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -667,8 +825,14 @@
       <c r="H4">
         <v>0.131908</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>0.12825700000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -687,8 +851,14 @@
       <c r="H5">
         <v>0.12608</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>0.116748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -707,8 +877,14 @@
       <c r="H6">
         <v>0.122331</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>8.3079E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -727,8 +903,14 @@
       <c r="H7">
         <v>9.7373000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7">
+        <v>7.6443999999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -747,8 +929,14 @@
       <c r="H8">
         <v>5.4740999999999998E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8">
+        <v>7.4452000000000004E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -767,8 +955,14 @@
       <c r="H9">
         <v>4.5010000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>7.0033999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -787,8 +981,14 @@
       <c r="H10">
         <v>4.0503999999999998E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10">
+        <v>6.7913000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -807,8 +1007,14 @@
       <c r="H11">
         <v>3.8263999999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11">
+        <v>5.3655000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -827,8 +1033,14 @@
       <c r="H12">
         <v>1.8796E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12">
+        <v>4.9013000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -846,6 +1058,12 @@
       </c>
       <c r="H13">
         <v>1.848E-2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13">
+        <v>4.6905000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>